<commit_message>
changement de pom packaging maven
</commit_message>
<xml_diff>
--- a/DOCUMENTATION/Sprint 2/Planing.xlsx
+++ b/DOCUMENTATION/Sprint 2/Planing.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="36" windowWidth="23256" windowHeight="9852"/>
+    <workbookView xWindow="0" yWindow="2436" windowWidth="16584" windowHeight="5460"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -224,13 +225,13 @@
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -540,7 +541,7 @@
   <dimension ref="A1:AK15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="4" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -553,55 +554,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="3" t="s">
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="3" t="s">
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="2" t="s">
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="3" t="s">
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="V1" s="4"/>
-      <c r="W1" s="4"/>
-      <c r="X1" s="4"/>
-      <c r="Y1" s="3" t="s">
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="Z1" s="4"/>
-      <c r="AA1" s="4"/>
+      <c r="Z1" s="3"/>
+      <c r="AA1" s="3"/>
       <c r="AB1" s="5"/>
-      <c r="AC1" s="2" t="s">
+      <c r="AC1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="AD1" s="2"/>
-      <c r="AE1" s="2"/>
-      <c r="AF1" s="2"/>
-      <c r="AG1" s="2"/>
-      <c r="AH1" s="3" t="s">
+      <c r="AD1" s="4"/>
+      <c r="AE1" s="4"/>
+      <c r="AF1" s="4"/>
+      <c r="AG1" s="4"/>
+      <c r="AH1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="AI1" s="4"/>
-      <c r="AJ1" s="4"/>
-      <c r="AK1" s="4"/>
+      <c r="AI1" s="3"/>
+      <c r="AJ1" s="3"/>
+      <c r="AK1" s="3"/>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -716,7 +717,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>100</v>
       </c>
@@ -733,7 +734,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="4" spans="1:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>200</v>
       </c>
@@ -767,7 +768,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="6" spans="1:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>400</v>
       </c>
@@ -784,7 +785,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>500</v>
       </c>
@@ -801,7 +802,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>510</v>
       </c>
@@ -818,7 +819,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>520</v>
       </c>
@@ -836,7 +837,7 @@
       </c>
     </row>
     <row r="10" spans="1:37" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>610</v>
       </c>

</xml_diff>